<commit_message>
Update Covid-19 National Mortality Model.xlsx
</commit_message>
<xml_diff>
--- a/Covid-19 National Mortality Model.xlsx
+++ b/Covid-19 National Mortality Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="180" windowWidth="17955" windowHeight="9435"/>
+    <workbookView xWindow="690" yWindow="180" windowWidth="17955" windowHeight="9435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Covid-19 Mortality" sheetId="2" r:id="rId1"/>
@@ -837,11 +837,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41686912"/>
-        <c:axId val="41688448"/>
+        <c:axId val="122807808"/>
+        <c:axId val="162930688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41686912"/>
+        <c:axId val="122807808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +851,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41688448"/>
+        <c:crossAx val="162930688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -859,7 +859,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41688448"/>
+        <c:axId val="162930688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +870,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41686912"/>
+        <c:crossAx val="122807808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1216,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>